<commit_message>
fertig bis auf Lippe
</commit_message>
<xml_diff>
--- a/German_Tales/Data/German_tales_FS.xlsx
+++ b/German_Tales/Data/German_tales_FS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81aa60b0b6324d95/Dokumente/GitHub/DWA/German_Tales/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="773" documentId="11_B99231273C39E9D1B8753BE6E77F10359AD05542" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E3EAC43-99F4-49B7-91AC-25E338E2ED27}"/>
+  <xr:revisionPtr revIDLastSave="839" documentId="11_B99231273C39E9D1B8753BE6E77F10359AD05542" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A477B37-5A3E-4CB7-BE49-9B89DB3AA8E6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10509" uniqueCount="2208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10550" uniqueCount="2235">
   <si>
     <t>ID</t>
   </si>
@@ -6644,6 +6644,87 @@
   </si>
   <si>
     <t>Nu scheint die Sonne so hell und klar.</t>
+  </si>
+  <si>
+    <t>Wat ki[e]kt us de Stärnkes so fröndlick an.</t>
+  </si>
+  <si>
+    <t>Was schaut uns der [?] so freundlich an.</t>
+  </si>
+  <si>
+    <t>Lambertus sall liäwen.</t>
+  </si>
+  <si>
+    <t>Lambertus soll leben.</t>
+  </si>
+  <si>
+    <t>Biuch,HW</t>
+  </si>
+  <si>
+    <t>erstmal die Koordinaten der Stadt Münster genommen. Im Text gibt es für liäwen die Anmerkung leben.</t>
+  </si>
+  <si>
+    <t>En Vertelserken van Bärndken van Gålen.</t>
+  </si>
+  <si>
+    <t>En Vertelserken van Uulenspeigel.</t>
+  </si>
+  <si>
+    <t>[?] von Eulenspiegel.</t>
+  </si>
+  <si>
+    <t>Timphot*.</t>
+  </si>
+  <si>
+    <t>Eckhut*.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buch  </t>
+  </si>
+  <si>
+    <t>De Schatzgriäwer.</t>
+  </si>
+  <si>
+    <t>Der Schatzgräber.</t>
+  </si>
+  <si>
+    <t>Ludgerus un de Geise*.</t>
+  </si>
+  <si>
+    <t>[Ludgerus] und die Gänse*.</t>
+  </si>
+  <si>
+    <t>De Kraomer in Tühr's Busk.</t>
+  </si>
+  <si>
+    <t>Lüdinkhusen.</t>
+  </si>
+  <si>
+    <t>Himmelfahrtsdag to Mönster.</t>
+  </si>
+  <si>
+    <t>Himmelfahrtstag zu Münster.</t>
+  </si>
+  <si>
+    <t>Volks- und Kinderlieder.</t>
+  </si>
+  <si>
+    <t>Wu ändert sick de Tid.</t>
+  </si>
+  <si>
+    <t>[Wie] ändert sich die Zeit.</t>
+  </si>
+  <si>
+    <t>Burenleed.</t>
+  </si>
+  <si>
+    <t>Bauernlied.</t>
+  </si>
+  <si>
+    <t>Kindergebetchen.</t>
+  </si>
+  <si>
+    <t>Ein Gebet, um zur rechten Zeit aufzuwachen.</t>
   </si>
 </sst>
 </file>
@@ -6665,7 +6746,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6684,6 +6765,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -6697,12 +6784,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7005,8 +7093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1397"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N807" workbookViewId="0">
-      <selection activeCell="R819" sqref="R819"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F345" sqref="F345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21765,13 +21853,13 @@
       </c>
     </row>
     <row r="329" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A329">
+      <c r="A329" s="5">
         <v>328</v>
       </c>
-      <c r="B329">
+      <c r="B329" s="5">
         <v>1</v>
       </c>
-      <c r="C329" t="s">
+      <c r="C329" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D329">
@@ -21812,13 +21900,13 @@
       </c>
     </row>
     <row r="330" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A330">
+      <c r="A330" s="5">
         <v>329</v>
       </c>
-      <c r="B330">
+      <c r="B330" s="5">
         <v>1</v>
       </c>
-      <c r="C330" t="s">
+      <c r="C330" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D330">
@@ -21859,13 +21947,13 @@
       </c>
     </row>
     <row r="331" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A331">
+      <c r="A331" s="5">
         <v>330</v>
       </c>
-      <c r="B331">
+      <c r="B331" s="5">
         <v>1</v>
       </c>
-      <c r="C331" t="s">
+      <c r="C331" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D331">
@@ -21906,13 +21994,13 @@
       </c>
     </row>
     <row r="332" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A332">
+      <c r="A332" s="5">
         <v>331</v>
       </c>
-      <c r="B332">
+      <c r="B332" s="5">
         <v>1</v>
       </c>
-      <c r="C332" t="s">
+      <c r="C332" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D332">
@@ -21953,13 +22041,13 @@
       </c>
     </row>
     <row r="333" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A333">
+      <c r="A333" s="5">
         <v>332</v>
       </c>
-      <c r="B333">
+      <c r="B333" s="5">
         <v>1</v>
       </c>
-      <c r="C333" t="s">
+      <c r="C333" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D333">
@@ -22000,13 +22088,13 @@
       </c>
     </row>
     <row r="334" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A334">
+      <c r="A334" s="5">
         <v>333</v>
       </c>
-      <c r="B334">
+      <c r="B334" s="5">
         <v>1</v>
       </c>
-      <c r="C334" t="s">
+      <c r="C334" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D334">
@@ -22047,13 +22135,13 @@
       </c>
     </row>
     <row r="335" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A335">
+      <c r="A335" s="5">
         <v>334</v>
       </c>
-      <c r="B335">
+      <c r="B335" s="5">
         <v>1</v>
       </c>
-      <c r="C335" t="s">
+      <c r="C335" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D335">
@@ -22094,13 +22182,13 @@
       </c>
     </row>
     <row r="336" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A336">
+      <c r="A336" s="5">
         <v>335</v>
       </c>
-      <c r="B336">
+      <c r="B336" s="5">
         <v>1</v>
       </c>
-      <c r="C336" t="s">
+      <c r="C336" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D336">
@@ -22141,13 +22229,13 @@
       </c>
     </row>
     <row r="337" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A337">
+      <c r="A337" s="5">
         <v>336</v>
       </c>
-      <c r="B337">
+      <c r="B337" s="5">
         <v>1</v>
       </c>
-      <c r="C337" t="s">
+      <c r="C337" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D337">
@@ -22188,13 +22276,13 @@
       </c>
     </row>
     <row r="338" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A338">
+      <c r="A338" s="5">
         <v>337</v>
       </c>
-      <c r="B338">
+      <c r="B338" s="5">
         <v>1</v>
       </c>
-      <c r="C338" t="s">
+      <c r="C338" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D338">
@@ -22235,13 +22323,13 @@
       </c>
     </row>
     <row r="339" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A339">
+      <c r="A339" s="5">
         <v>338</v>
       </c>
-      <c r="B339">
+      <c r="B339" s="5">
         <v>1</v>
       </c>
-      <c r="C339" t="s">
+      <c r="C339" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D339">
@@ -22282,13 +22370,13 @@
       </c>
     </row>
     <row r="340" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A340">
+      <c r="A340" s="5">
         <v>339</v>
       </c>
-      <c r="B340">
+      <c r="B340" s="5">
         <v>1</v>
       </c>
-      <c r="C340" t="s">
+      <c r="C340" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D340">
@@ -22329,13 +22417,13 @@
       </c>
     </row>
     <row r="341" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A341">
+      <c r="A341" s="5">
         <v>340</v>
       </c>
-      <c r="B341">
+      <c r="B341" s="5">
         <v>1</v>
       </c>
-      <c r="C341" t="s">
+      <c r="C341" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D341">
@@ -22376,13 +22464,13 @@
       </c>
     </row>
     <row r="342" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A342">
+      <c r="A342" s="5">
         <v>341</v>
       </c>
-      <c r="B342">
+      <c r="B342" s="5">
         <v>1</v>
       </c>
-      <c r="C342" t="s">
+      <c r="C342" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D342">
@@ -22423,13 +22511,13 @@
       </c>
     </row>
     <row r="343" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A343">
+      <c r="A343" s="5">
         <v>342</v>
       </c>
-      <c r="B343">
+      <c r="B343" s="5">
         <v>1</v>
       </c>
-      <c r="C343" t="s">
+      <c r="C343" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D343">
@@ -22470,13 +22558,13 @@
       </c>
     </row>
     <row r="344" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A344">
+      <c r="A344" s="5">
         <v>343</v>
       </c>
-      <c r="B344">
+      <c r="B344" s="5">
         <v>1</v>
       </c>
-      <c r="C344" t="s">
+      <c r="C344" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D344">
@@ -22517,13 +22605,13 @@
       </c>
     </row>
     <row r="345" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A345">
+      <c r="A345" s="5">
         <v>344</v>
       </c>
-      <c r="B345">
+      <c r="B345" s="5">
         <v>1</v>
       </c>
-      <c r="C345" t="s">
+      <c r="C345" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D345">
@@ -22564,13 +22652,13 @@
       </c>
     </row>
     <row r="346" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A346">
+      <c r="A346" s="5">
         <v>345</v>
       </c>
-      <c r="B346">
+      <c r="B346" s="5">
         <v>1</v>
       </c>
-      <c r="C346" t="s">
+      <c r="C346" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D346">
@@ -22611,13 +22699,13 @@
       </c>
     </row>
     <row r="347" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A347">
+      <c r="A347" s="5">
         <v>346</v>
       </c>
-      <c r="B347">
+      <c r="B347" s="5">
         <v>1</v>
       </c>
-      <c r="C347" t="s">
+      <c r="C347" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D347">
@@ -22658,13 +22746,13 @@
       </c>
     </row>
     <row r="348" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A348">
+      <c r="A348" s="5">
         <v>347</v>
       </c>
-      <c r="B348">
+      <c r="B348" s="5">
         <v>1</v>
       </c>
-      <c r="C348" t="s">
+      <c r="C348" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D348">
@@ -22705,13 +22793,13 @@
       </c>
     </row>
     <row r="349" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A349">
+      <c r="A349" s="5">
         <v>348</v>
       </c>
-      <c r="B349">
+      <c r="B349" s="5">
         <v>1</v>
       </c>
-      <c r="C349" t="s">
+      <c r="C349" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D349">
@@ -22752,13 +22840,13 @@
       </c>
     </row>
     <row r="350" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A350">
+      <c r="A350" s="5">
         <v>349</v>
       </c>
-      <c r="B350">
+      <c r="B350" s="5">
         <v>1</v>
       </c>
-      <c r="C350" t="s">
+      <c r="C350" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D350">
@@ -22799,13 +22887,13 @@
       </c>
     </row>
     <row r="351" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A351">
+      <c r="A351" s="5">
         <v>350</v>
       </c>
-      <c r="B351">
+      <c r="B351" s="5">
         <v>1</v>
       </c>
-      <c r="C351" t="s">
+      <c r="C351" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D351">
@@ -22846,13 +22934,13 @@
       </c>
     </row>
     <row r="352" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A352">
+      <c r="A352" s="5">
         <v>351</v>
       </c>
-      <c r="B352">
+      <c r="B352" s="5">
         <v>1</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C352" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D352">
@@ -22893,13 +22981,13 @@
       </c>
     </row>
     <row r="353" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A353">
+      <c r="A353" s="5">
         <v>352</v>
       </c>
-      <c r="B353">
+      <c r="B353" s="5">
         <v>1</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C353" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D353">
@@ -22940,13 +23028,13 @@
       </c>
     </row>
     <row r="354" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A354">
+      <c r="A354" s="5">
         <v>353</v>
       </c>
-      <c r="B354">
+      <c r="B354" s="5">
         <v>1</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C354" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D354">
@@ -22987,13 +23075,13 @@
       </c>
     </row>
     <row r="355" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A355">
+      <c r="A355" s="5">
         <v>354</v>
       </c>
-      <c r="B355">
+      <c r="B355" s="5">
         <v>1</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C355" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D355">
@@ -23034,13 +23122,13 @@
       </c>
     </row>
     <row r="356" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A356">
+      <c r="A356" s="5">
         <v>355</v>
       </c>
-      <c r="B356">
+      <c r="B356" s="5">
         <v>1</v>
       </c>
-      <c r="C356" t="s">
+      <c r="C356" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D356">
@@ -23081,13 +23169,13 @@
       </c>
     </row>
     <row r="357" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A357">
+      <c r="A357" s="5">
         <v>356</v>
       </c>
-      <c r="B357">
+      <c r="B357" s="5">
         <v>1</v>
       </c>
-      <c r="C357" t="s">
+      <c r="C357" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D357">
@@ -23128,13 +23216,13 @@
       </c>
     </row>
     <row r="358" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A358">
+      <c r="A358" s="5">
         <v>357</v>
       </c>
-      <c r="B358">
+      <c r="B358" s="5">
         <v>1</v>
       </c>
-      <c r="C358" t="s">
+      <c r="C358" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D358">
@@ -23175,13 +23263,13 @@
       </c>
     </row>
     <row r="359" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A359">
+      <c r="A359" s="5">
         <v>358</v>
       </c>
-      <c r="B359">
+      <c r="B359" s="5">
         <v>1</v>
       </c>
-      <c r="C359" t="s">
+      <c r="C359" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D359">
@@ -23222,13 +23310,13 @@
       </c>
     </row>
     <row r="360" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A360">
+      <c r="A360" s="5">
         <v>359</v>
       </c>
-      <c r="B360">
+      <c r="B360" s="5">
         <v>1</v>
       </c>
-      <c r="C360" t="s">
+      <c r="C360" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D360">
@@ -23269,13 +23357,13 @@
       </c>
     </row>
     <row r="361" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A361">
+      <c r="A361" s="5">
         <v>360</v>
       </c>
-      <c r="B361">
+      <c r="B361" s="5">
         <v>1</v>
       </c>
-      <c r="C361" t="s">
+      <c r="C361" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D361">
@@ -23316,13 +23404,13 @@
       </c>
     </row>
     <row r="362" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A362">
+      <c r="A362" s="5">
         <v>361</v>
       </c>
-      <c r="B362">
+      <c r="B362" s="5">
         <v>1</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C362" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D362">
@@ -23363,13 +23451,13 @@
       </c>
     </row>
     <row r="363" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A363">
+      <c r="A363" s="5">
         <v>362</v>
       </c>
-      <c r="B363">
+      <c r="B363" s="5">
         <v>1</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C363" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D363">
@@ -23410,13 +23498,13 @@
       </c>
     </row>
     <row r="364" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A364">
+      <c r="A364" s="5">
         <v>363</v>
       </c>
-      <c r="B364">
+      <c r="B364" s="5">
         <v>1</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C364" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D364">
@@ -23457,13 +23545,13 @@
       </c>
     </row>
     <row r="365" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A365">
+      <c r="A365" s="5">
         <v>364</v>
       </c>
-      <c r="B365">
+      <c r="B365" s="5">
         <v>1</v>
       </c>
-      <c r="C365" t="s">
+      <c r="C365" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D365">
@@ -23504,13 +23592,13 @@
       </c>
     </row>
     <row r="366" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A366">
+      <c r="A366" s="5">
         <v>365</v>
       </c>
-      <c r="B366">
+      <c r="B366" s="5">
         <v>1</v>
       </c>
-      <c r="C366" t="s">
+      <c r="C366" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D366">
@@ -23551,13 +23639,13 @@
       </c>
     </row>
     <row r="367" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A367">
+      <c r="A367" s="5">
         <v>366</v>
       </c>
-      <c r="B367">
+      <c r="B367" s="5">
         <v>1</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C367" s="5" t="s">
         <v>614</v>
       </c>
       <c r="D367">
@@ -43393,6 +43481,15 @@
       <c r="P820" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q820" t="s">
+        <v>2208</v>
+      </c>
+      <c r="R820" t="s">
+        <v>2209</v>
+      </c>
+      <c r="S820" t="s">
+        <v>1996</v>
+      </c>
       <c r="T820" t="s">
         <v>2197</v>
       </c>
@@ -43443,8 +43540,17 @@
       <c r="P821" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q821" t="s">
+        <v>2210</v>
+      </c>
+      <c r="R821" t="s">
+        <v>2211</v>
+      </c>
+      <c r="S821" t="s">
+        <v>2212</v>
+      </c>
       <c r="T821" t="s">
-        <v>2197</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="822" spans="1:20" x14ac:dyDescent="0.25">
@@ -43493,6 +43599,15 @@
       <c r="P822" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q822" t="s">
+        <v>2214</v>
+      </c>
+      <c r="R822">
+        <v>999</v>
+      </c>
+      <c r="S822">
+        <v>999</v>
+      </c>
       <c r="T822" t="s">
         <v>2197</v>
       </c>
@@ -43543,6 +43658,15 @@
       <c r="P823" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q823" t="s">
+        <v>2215</v>
+      </c>
+      <c r="R823" t="s">
+        <v>2216</v>
+      </c>
+      <c r="S823" t="s">
+        <v>1996</v>
+      </c>
       <c r="T823" t="s">
         <v>2197</v>
       </c>
@@ -43593,6 +43717,15 @@
       <c r="P824" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q824" t="s">
+        <v>2217</v>
+      </c>
+      <c r="R824" t="s">
+        <v>2218</v>
+      </c>
+      <c r="S824" t="s">
+        <v>2219</v>
+      </c>
       <c r="T824" t="s">
         <v>2197</v>
       </c>
@@ -43643,6 +43776,15 @@
       <c r="P825" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q825" t="s">
+        <v>2220</v>
+      </c>
+      <c r="R825" t="s">
+        <v>2221</v>
+      </c>
+      <c r="S825" t="s">
+        <v>1996</v>
+      </c>
       <c r="T825" t="s">
         <v>2197</v>
       </c>
@@ -43693,6 +43835,15 @@
       <c r="P826" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q826" t="s">
+        <v>2222</v>
+      </c>
+      <c r="R826" t="s">
+        <v>2223</v>
+      </c>
+      <c r="S826" t="s">
+        <v>2009</v>
+      </c>
       <c r="T826" t="s">
         <v>2197</v>
       </c>
@@ -43743,6 +43894,15 @@
       <c r="P827" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q827" t="s">
+        <v>2224</v>
+      </c>
+      <c r="R827">
+        <v>999</v>
+      </c>
+      <c r="S827">
+        <v>999</v>
+      </c>
       <c r="T827" t="s">
         <v>2197</v>
       </c>
@@ -43793,6 +43953,15 @@
       <c r="P828" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q828" t="s">
+        <v>2225</v>
+      </c>
+      <c r="R828" t="s">
+        <v>2225</v>
+      </c>
+      <c r="S828" t="s">
+        <v>1996</v>
+      </c>
       <c r="T828" t="s">
         <v>2197</v>
       </c>
@@ -43843,18 +44012,27 @@
       <c r="P829" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q829" t="s">
+        <v>2226</v>
+      </c>
+      <c r="R829" t="s">
+        <v>2227</v>
+      </c>
+      <c r="S829" t="s">
+        <v>1996</v>
+      </c>
       <c r="T829" t="s">
         <v>2197</v>
       </c>
     </row>
     <row r="830" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A830">
+      <c r="A830" s="5">
         <v>829</v>
       </c>
-      <c r="B830">
+      <c r="B830" s="5">
         <v>1</v>
       </c>
-      <c r="C830" t="s">
+      <c r="C830" s="5" t="s">
         <v>1344</v>
       </c>
       <c r="D830">
@@ -43893,18 +44071,27 @@
       <c r="P830" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q830" t="s">
+        <v>2228</v>
+      </c>
+      <c r="R830" t="s">
+        <v>2228</v>
+      </c>
+      <c r="S830" t="s">
+        <v>1996</v>
+      </c>
       <c r="T830" t="s">
         <v>2197</v>
       </c>
     </row>
     <row r="831" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A831">
+      <c r="A831" s="5">
         <v>830</v>
       </c>
-      <c r="B831">
+      <c r="B831" s="5">
         <v>1</v>
       </c>
-      <c r="C831" t="s">
+      <c r="C831" s="5" t="s">
         <v>1344</v>
       </c>
       <c r="D831">
@@ -43943,18 +44130,27 @@
       <c r="P831" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q831" t="s">
+        <v>2229</v>
+      </c>
+      <c r="R831" t="s">
+        <v>2230</v>
+      </c>
+      <c r="S831" t="s">
+        <v>1996</v>
+      </c>
       <c r="T831" t="s">
         <v>2197</v>
       </c>
     </row>
     <row r="832" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A832">
+      <c r="A832" s="5">
         <v>831</v>
       </c>
-      <c r="B832">
+      <c r="B832" s="5">
         <v>1</v>
       </c>
-      <c r="C832" t="s">
+      <c r="C832" s="5" t="s">
         <v>1344</v>
       </c>
       <c r="D832">
@@ -43993,18 +44189,27 @@
       <c r="P832" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q832" t="s">
+        <v>2231</v>
+      </c>
+      <c r="R832" t="s">
+        <v>2232</v>
+      </c>
+      <c r="S832" t="s">
+        <v>1996</v>
+      </c>
       <c r="T832" t="s">
         <v>2197</v>
       </c>
     </row>
     <row r="833" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A833">
+      <c r="A833" s="5">
         <v>832</v>
       </c>
-      <c r="B833">
+      <c r="B833" s="5">
         <v>1</v>
       </c>
-      <c r="C833" t="s">
+      <c r="C833" s="5" t="s">
         <v>1344</v>
       </c>
       <c r="D833">
@@ -44043,18 +44248,27 @@
       <c r="P833" s="4" t="s">
         <v>2199</v>
       </c>
+      <c r="Q833" t="s">
+        <v>2233</v>
+      </c>
+      <c r="R833" t="s">
+        <v>2233</v>
+      </c>
+      <c r="S833" t="s">
+        <v>1996</v>
+      </c>
       <c r="T833" t="s">
         <v>2197</v>
       </c>
     </row>
     <row r="834" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A834">
+      <c r="A834" s="5">
         <v>833</v>
       </c>
-      <c r="B834">
+      <c r="B834" s="5">
         <v>1</v>
       </c>
-      <c r="C834" t="s">
+      <c r="C834" s="5" t="s">
         <v>1344</v>
       </c>
       <c r="D834">
@@ -44092,6 +44306,15 @@
       </c>
       <c r="P834" s="4" t="s">
         <v>2199</v>
+      </c>
+      <c r="Q834" t="s">
+        <v>2234</v>
+      </c>
+      <c r="R834" t="s">
+        <v>2234</v>
+      </c>
+      <c r="S834" t="s">
+        <v>1996</v>
       </c>
       <c r="T834" t="s">
         <v>2197</v>

</xml_diff>